<commit_message>
Fixed some bugs and addes template importer tests
</commit_message>
<xml_diff>
--- a/backend/fms_core/tests/valid_templates/Project_link_samples_v4_0_0.xlsx
+++ b/backend/fms_core/tests/valid_templates/Project_link_samples_v4_0_0.xlsx
@@ -12,7 +12,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" uniqueCount="25">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" uniqueCount="28">
   <si>
     <t>Project link samples Template</t>
   </si>
@@ -86,7 +86,16 @@
     <t>Add to study</t>
   </si>
   <si>
+    <t>A</t>
+  </si>
+  <si>
+    <t>3</t>
+  </si>
+  <si>
     <t>Remove from study</t>
+  </si>
+  <si>
+    <t>B</t>
   </si>
 </sst>
 </file>
@@ -263,7 +272,7 @@
       <alignment vertical="bottom"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="24">
+  <cellXfs count="25">
     <xf numFmtId="0" fontId="0" applyNumberFormat="0" applyFont="1" applyFill="0" applyBorder="0" applyAlignment="1" applyProtection="0">
       <alignment vertical="bottom"/>
     </xf>
@@ -326,6 +335,9 @@
     </xf>
     <xf numFmtId="0" fontId="8" fillId="2" borderId="1" applyNumberFormat="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
       <alignment vertical="bottom"/>
+    </xf>
+    <xf numFmtId="49" fontId="8" fillId="2" borderId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
+      <alignment horizontal="left" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="8" fillId="2" borderId="1" applyNumberFormat="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
       <alignment horizontal="center" vertical="center"/>
@@ -1610,37 +1622,69 @@
       <c r="H12" s="20"/>
     </row>
     <row r="13" ht="13.5" customHeight="1">
-      <c r="A13" s="21"/>
-      <c r="B13" s="18"/>
-      <c r="C13" s="19"/>
+      <c r="A13" t="s" s="18">
+        <v>23</v>
+      </c>
+      <c r="B13" t="s" s="21">
+        <v>13</v>
+      </c>
+      <c r="C13" t="s" s="19">
+        <v>24</v>
+      </c>
       <c r="D13" s="19"/>
-      <c r="E13" s="19"/>
-      <c r="F13" s="19"/>
+      <c r="E13" t="s" s="19">
+        <v>14</v>
+      </c>
+      <c r="F13" t="s" s="19">
+        <v>15</v>
+      </c>
       <c r="G13" s="19"/>
       <c r="H13" s="20"/>
     </row>
     <row r="14" ht="13.5" customHeight="1">
-      <c r="A14" s="21"/>
-      <c r="B14" s="18"/>
-      <c r="C14" s="19"/>
-      <c r="D14" s="19"/>
-      <c r="E14" s="19"/>
-      <c r="F14" s="19"/>
+      <c r="A14" t="s" s="18">
+        <v>23</v>
+      </c>
+      <c r="B14" t="s" s="21">
+        <v>13</v>
+      </c>
+      <c r="C14" t="s" s="19">
+        <v>24</v>
+      </c>
+      <c r="D14" t="s" s="19">
+        <v>25</v>
+      </c>
+      <c r="E14" t="s" s="19">
+        <v>14</v>
+      </c>
+      <c r="F14" t="s" s="19">
+        <v>15</v>
+      </c>
       <c r="G14" s="19"/>
       <c r="H14" s="20"/>
     </row>
     <row r="15" ht="13.5" customHeight="1">
-      <c r="A15" s="21"/>
-      <c r="B15" s="18"/>
-      <c r="C15" s="19"/>
+      <c r="A15" t="s" s="18">
+        <v>26</v>
+      </c>
+      <c r="B15" t="s" s="21">
+        <v>13</v>
+      </c>
+      <c r="C15" t="s" s="19">
+        <v>27</v>
+      </c>
       <c r="D15" s="19"/>
-      <c r="E15" s="19"/>
-      <c r="F15" s="19"/>
+      <c r="E15" t="s" s="19">
+        <v>21</v>
+      </c>
+      <c r="F15" t="s" s="19">
+        <v>22</v>
+      </c>
       <c r="G15" s="19"/>
       <c r="H15" s="20"/>
     </row>
     <row r="16" ht="13.5" customHeight="1">
-      <c r="A16" s="21"/>
+      <c r="A16" s="22"/>
       <c r="B16" s="18"/>
       <c r="C16" s="19"/>
       <c r="D16" s="19"/>
@@ -1650,7 +1694,7 @@
       <c r="H16" s="20"/>
     </row>
     <row r="17" ht="13.5" customHeight="1">
-      <c r="A17" s="21"/>
+      <c r="A17" s="22"/>
       <c r="B17" s="18"/>
       <c r="C17" s="19"/>
       <c r="D17" s="19"/>
@@ -1660,7 +1704,7 @@
       <c r="H17" s="20"/>
     </row>
     <row r="18" ht="13.5" customHeight="1">
-      <c r="A18" s="21"/>
+      <c r="A18" s="22"/>
       <c r="B18" s="18"/>
       <c r="C18" s="19"/>
       <c r="D18" s="19"/>
@@ -1670,7 +1714,7 @@
       <c r="H18" s="20"/>
     </row>
     <row r="19" ht="13.5" customHeight="1">
-      <c r="A19" s="21"/>
+      <c r="A19" s="22"/>
       <c r="B19" s="18"/>
       <c r="C19" s="19"/>
       <c r="D19" s="19"/>
@@ -1680,7 +1724,7 @@
       <c r="H19" s="20"/>
     </row>
     <row r="20" ht="13.5" customHeight="1">
-      <c r="A20" s="21"/>
+      <c r="A20" s="22"/>
       <c r="B20" s="18"/>
       <c r="C20" s="19"/>
       <c r="D20" s="19"/>
@@ -1690,7 +1734,7 @@
       <c r="H20" s="20"/>
     </row>
     <row r="21" ht="13.5" customHeight="1">
-      <c r="A21" s="21"/>
+      <c r="A21" s="22"/>
       <c r="B21" s="18"/>
       <c r="C21" s="19"/>
       <c r="D21" s="19"/>
@@ -1700,7 +1744,7 @@
       <c r="H21" s="20"/>
     </row>
     <row r="22" ht="15.75" customHeight="1">
-      <c r="A22" s="21"/>
+      <c r="A22" s="22"/>
       <c r="B22" s="18"/>
       <c r="C22" s="19"/>
       <c r="D22" s="19"/>
@@ -1710,7 +1754,7 @@
       <c r="H22" s="20"/>
     </row>
     <row r="23" ht="15.75" customHeight="1">
-      <c r="A23" s="21"/>
+      <c r="A23" s="22"/>
       <c r="B23" s="18"/>
       <c r="C23" s="19"/>
       <c r="D23" s="19"/>
@@ -1720,7 +1764,7 @@
       <c r="H23" s="20"/>
     </row>
     <row r="24" ht="15.75" customHeight="1">
-      <c r="A24" s="21"/>
+      <c r="A24" s="22"/>
       <c r="B24" s="18"/>
       <c r="C24" s="19"/>
       <c r="D24" s="19"/>
@@ -1730,7 +1774,7 @@
       <c r="H24" s="20"/>
     </row>
     <row r="25" ht="15.75" customHeight="1">
-      <c r="A25" s="21"/>
+      <c r="A25" s="22"/>
       <c r="B25" s="18"/>
       <c r="C25" s="19"/>
       <c r="D25" s="19"/>
@@ -1740,7 +1784,7 @@
       <c r="H25" s="20"/>
     </row>
     <row r="26" ht="15.75" customHeight="1">
-      <c r="A26" s="21"/>
+      <c r="A26" s="22"/>
       <c r="B26" s="18"/>
       <c r="C26" s="19"/>
       <c r="D26" s="19"/>
@@ -1750,7 +1794,7 @@
       <c r="H26" s="20"/>
     </row>
     <row r="27" ht="15.75" customHeight="1">
-      <c r="A27" s="21"/>
+      <c r="A27" s="22"/>
       <c r="B27" s="18"/>
       <c r="C27" s="19"/>
       <c r="D27" s="19"/>
@@ -1760,7 +1804,7 @@
       <c r="H27" s="20"/>
     </row>
     <row r="28" ht="15.75" customHeight="1">
-      <c r="A28" s="21"/>
+      <c r="A28" s="22"/>
       <c r="B28" s="18"/>
       <c r="C28" s="19"/>
       <c r="D28" s="19"/>
@@ -1770,7 +1814,7 @@
       <c r="H28" s="20"/>
     </row>
     <row r="29" ht="15.75" customHeight="1">
-      <c r="A29" s="21"/>
+      <c r="A29" s="22"/>
       <c r="B29" s="18"/>
       <c r="C29" s="19"/>
       <c r="D29" s="19"/>
@@ -1780,7 +1824,7 @@
       <c r="H29" s="20"/>
     </row>
     <row r="30" ht="15.75" customHeight="1">
-      <c r="A30" s="21"/>
+      <c r="A30" s="22"/>
       <c r="B30" s="18"/>
       <c r="C30" s="19"/>
       <c r="D30" s="19"/>
@@ -1790,7 +1834,7 @@
       <c r="H30" s="20"/>
     </row>
     <row r="31" ht="15.75" customHeight="1">
-      <c r="A31" s="21"/>
+      <c r="A31" s="22"/>
       <c r="B31" s="18"/>
       <c r="C31" s="19"/>
       <c r="D31" s="19"/>
@@ -1800,7 +1844,7 @@
       <c r="H31" s="20"/>
     </row>
     <row r="32" ht="15.75" customHeight="1">
-      <c r="A32" s="21"/>
+      <c r="A32" s="22"/>
       <c r="B32" s="18"/>
       <c r="C32" s="19"/>
       <c r="D32" s="19"/>
@@ -1810,7 +1854,7 @@
       <c r="H32" s="20"/>
     </row>
     <row r="33" ht="15.75" customHeight="1">
-      <c r="A33" s="21"/>
+      <c r="A33" s="22"/>
       <c r="B33" s="18"/>
       <c r="C33" s="19"/>
       <c r="D33" s="19"/>
@@ -1820,7 +1864,7 @@
       <c r="H33" s="20"/>
     </row>
     <row r="34" ht="15.75" customHeight="1">
-      <c r="A34" s="21"/>
+      <c r="A34" s="22"/>
       <c r="B34" s="18"/>
       <c r="C34" s="19"/>
       <c r="D34" s="19"/>
@@ -1830,7 +1874,7 @@
       <c r="H34" s="20"/>
     </row>
     <row r="35" ht="15.75" customHeight="1">
-      <c r="A35" s="21"/>
+      <c r="A35" s="22"/>
       <c r="B35" s="18"/>
       <c r="C35" s="19"/>
       <c r="D35" s="19"/>
@@ -1840,7 +1884,7 @@
       <c r="H35" s="20"/>
     </row>
     <row r="36" ht="15.75" customHeight="1">
-      <c r="A36" s="21"/>
+      <c r="A36" s="22"/>
       <c r="B36" s="18"/>
       <c r="C36" s="19"/>
       <c r="D36" s="19"/>
@@ -1850,7 +1894,7 @@
       <c r="H36" s="20"/>
     </row>
     <row r="37" ht="15.75" customHeight="1">
-      <c r="A37" s="21"/>
+      <c r="A37" s="22"/>
       <c r="B37" s="18"/>
       <c r="C37" s="19"/>
       <c r="D37" s="19"/>
@@ -1860,7 +1904,7 @@
       <c r="H37" s="20"/>
     </row>
     <row r="38" ht="15.75" customHeight="1">
-      <c r="A38" s="21"/>
+      <c r="A38" s="22"/>
       <c r="B38" s="18"/>
       <c r="C38" s="19"/>
       <c r="D38" s="19"/>
@@ -1870,7 +1914,7 @@
       <c r="H38" s="20"/>
     </row>
     <row r="39" ht="15.75" customHeight="1">
-      <c r="A39" s="21"/>
+      <c r="A39" s="22"/>
       <c r="B39" s="18"/>
       <c r="C39" s="19"/>
       <c r="D39" s="19"/>
@@ -1880,7 +1924,7 @@
       <c r="H39" s="20"/>
     </row>
     <row r="40" ht="15.75" customHeight="1">
-      <c r="A40" s="21"/>
+      <c r="A40" s="22"/>
       <c r="B40" s="18"/>
       <c r="C40" s="19"/>
       <c r="D40" s="19"/>
@@ -1890,7 +1934,7 @@
       <c r="H40" s="20"/>
     </row>
     <row r="41" ht="15.75" customHeight="1">
-      <c r="A41" s="21"/>
+      <c r="A41" s="22"/>
       <c r="B41" s="18"/>
       <c r="C41" s="19"/>
       <c r="D41" s="19"/>
@@ -1900,7 +1944,7 @@
       <c r="H41" s="20"/>
     </row>
     <row r="42" ht="15.75" customHeight="1">
-      <c r="A42" s="21"/>
+      <c r="A42" s="22"/>
       <c r="B42" s="18"/>
       <c r="C42" s="19"/>
       <c r="D42" s="19"/>
@@ -1910,7 +1954,7 @@
       <c r="H42" s="20"/>
     </row>
     <row r="43" ht="15.75" customHeight="1">
-      <c r="A43" s="21"/>
+      <c r="A43" s="22"/>
       <c r="B43" s="18"/>
       <c r="C43" s="19"/>
       <c r="D43" s="19"/>
@@ -1920,7 +1964,7 @@
       <c r="H43" s="20"/>
     </row>
     <row r="44" ht="15.75" customHeight="1">
-      <c r="A44" s="21"/>
+      <c r="A44" s="22"/>
       <c r="B44" s="18"/>
       <c r="C44" s="19"/>
       <c r="D44" s="19"/>
@@ -1930,7 +1974,7 @@
       <c r="H44" s="20"/>
     </row>
     <row r="45" ht="15.75" customHeight="1">
-      <c r="A45" s="21"/>
+      <c r="A45" s="22"/>
       <c r="B45" s="18"/>
       <c r="C45" s="19"/>
       <c r="D45" s="19"/>
@@ -1940,7 +1984,7 @@
       <c r="H45" s="20"/>
     </row>
     <row r="46" ht="15.75" customHeight="1">
-      <c r="A46" s="21"/>
+      <c r="A46" s="22"/>
       <c r="B46" s="18"/>
       <c r="C46" s="19"/>
       <c r="D46" s="19"/>
@@ -1950,7 +1994,7 @@
       <c r="H46" s="20"/>
     </row>
     <row r="47" ht="15.75" customHeight="1">
-      <c r="A47" s="21"/>
+      <c r="A47" s="22"/>
       <c r="B47" s="18"/>
       <c r="C47" s="19"/>
       <c r="D47" s="19"/>
@@ -1960,7 +2004,7 @@
       <c r="H47" s="20"/>
     </row>
     <row r="48" ht="15.75" customHeight="1">
-      <c r="A48" s="21"/>
+      <c r="A48" s="22"/>
       <c r="B48" s="18"/>
       <c r="C48" s="19"/>
       <c r="D48" s="19"/>
@@ -1970,7 +2014,7 @@
       <c r="H48" s="20"/>
     </row>
     <row r="49" ht="15.75" customHeight="1">
-      <c r="A49" s="21"/>
+      <c r="A49" s="22"/>
       <c r="B49" s="18"/>
       <c r="C49" s="19"/>
       <c r="D49" s="19"/>
@@ -1980,7 +2024,7 @@
       <c r="H49" s="20"/>
     </row>
     <row r="50" ht="15.75" customHeight="1">
-      <c r="A50" s="21"/>
+      <c r="A50" s="22"/>
       <c r="B50" s="18"/>
       <c r="C50" s="19"/>
       <c r="D50" s="19"/>
@@ -1990,7 +2034,7 @@
       <c r="H50" s="20"/>
     </row>
     <row r="51" ht="15.75" customHeight="1">
-      <c r="A51" s="21"/>
+      <c r="A51" s="22"/>
       <c r="B51" s="18"/>
       <c r="C51" s="19"/>
       <c r="D51" s="19"/>
@@ -2000,7 +2044,7 @@
       <c r="H51" s="20"/>
     </row>
     <row r="52" ht="15.75" customHeight="1">
-      <c r="A52" s="21"/>
+      <c r="A52" s="22"/>
       <c r="B52" s="18"/>
       <c r="C52" s="19"/>
       <c r="D52" s="19"/>
@@ -2010,7 +2054,7 @@
       <c r="H52" s="20"/>
     </row>
     <row r="53" ht="15.75" customHeight="1">
-      <c r="A53" s="21"/>
+      <c r="A53" s="22"/>
       <c r="B53" s="18"/>
       <c r="C53" s="19"/>
       <c r="D53" s="19"/>
@@ -2020,7 +2064,7 @@
       <c r="H53" s="20"/>
     </row>
     <row r="54" ht="15.75" customHeight="1">
-      <c r="A54" s="21"/>
+      <c r="A54" s="22"/>
       <c r="B54" s="18"/>
       <c r="C54" s="19"/>
       <c r="D54" s="19"/>
@@ -2030,7 +2074,7 @@
       <c r="H54" s="20"/>
     </row>
     <row r="55" ht="15.75" customHeight="1">
-      <c r="A55" s="21"/>
+      <c r="A55" s="22"/>
       <c r="B55" s="18"/>
       <c r="C55" s="19"/>
       <c r="D55" s="19"/>
@@ -2040,7 +2084,7 @@
       <c r="H55" s="20"/>
     </row>
     <row r="56" ht="15.75" customHeight="1">
-      <c r="A56" s="21"/>
+      <c r="A56" s="22"/>
       <c r="B56" s="18"/>
       <c r="C56" s="19"/>
       <c r="D56" s="19"/>
@@ -2050,7 +2094,7 @@
       <c r="H56" s="20"/>
     </row>
     <row r="57" ht="15.75" customHeight="1">
-      <c r="A57" s="21"/>
+      <c r="A57" s="22"/>
       <c r="B57" s="18"/>
       <c r="C57" s="19"/>
       <c r="D57" s="19"/>
@@ -2060,7 +2104,7 @@
       <c r="H57" s="20"/>
     </row>
     <row r="58" ht="15.75" customHeight="1">
-      <c r="A58" s="21"/>
+      <c r="A58" s="22"/>
       <c r="B58" s="18"/>
       <c r="C58" s="19"/>
       <c r="D58" s="19"/>
@@ -2070,7 +2114,7 @@
       <c r="H58" s="20"/>
     </row>
     <row r="59" ht="15.75" customHeight="1">
-      <c r="A59" s="21"/>
+      <c r="A59" s="22"/>
       <c r="B59" s="18"/>
       <c r="C59" s="19"/>
       <c r="D59" s="19"/>
@@ -2080,7 +2124,7 @@
       <c r="H59" s="20"/>
     </row>
     <row r="60" ht="15.75" customHeight="1">
-      <c r="A60" s="21"/>
+      <c r="A60" s="22"/>
       <c r="B60" s="18"/>
       <c r="C60" s="19"/>
       <c r="D60" s="19"/>
@@ -2090,7 +2134,7 @@
       <c r="H60" s="20"/>
     </row>
     <row r="61" ht="15.75" customHeight="1">
-      <c r="A61" s="21"/>
+      <c r="A61" s="22"/>
       <c r="B61" s="18"/>
       <c r="C61" s="19"/>
       <c r="D61" s="19"/>
@@ -2100,7 +2144,7 @@
       <c r="H61" s="20"/>
     </row>
     <row r="62" ht="15.75" customHeight="1">
-      <c r="A62" s="21"/>
+      <c r="A62" s="22"/>
       <c r="B62" s="18"/>
       <c r="C62" s="19"/>
       <c r="D62" s="19"/>
@@ -2110,7 +2154,7 @@
       <c r="H62" s="20"/>
     </row>
     <row r="63" ht="15.75" customHeight="1">
-      <c r="A63" s="21"/>
+      <c r="A63" s="22"/>
       <c r="B63" s="18"/>
       <c r="C63" s="19"/>
       <c r="D63" s="19"/>
@@ -2120,7 +2164,7 @@
       <c r="H63" s="20"/>
     </row>
     <row r="64" ht="15.75" customHeight="1">
-      <c r="A64" s="21"/>
+      <c r="A64" s="22"/>
       <c r="B64" s="18"/>
       <c r="C64" s="19"/>
       <c r="D64" s="19"/>
@@ -2130,7 +2174,7 @@
       <c r="H64" s="20"/>
     </row>
     <row r="65" ht="15.75" customHeight="1">
-      <c r="A65" s="21"/>
+      <c r="A65" s="22"/>
       <c r="B65" s="18"/>
       <c r="C65" s="19"/>
       <c r="D65" s="19"/>
@@ -2140,7 +2184,7 @@
       <c r="H65" s="20"/>
     </row>
     <row r="66" ht="15.75" customHeight="1">
-      <c r="A66" s="21"/>
+      <c r="A66" s="22"/>
       <c r="B66" s="18"/>
       <c r="C66" s="19"/>
       <c r="D66" s="19"/>
@@ -2150,7 +2194,7 @@
       <c r="H66" s="20"/>
     </row>
     <row r="67" ht="15.75" customHeight="1">
-      <c r="A67" s="21"/>
+      <c r="A67" s="22"/>
       <c r="B67" s="18"/>
       <c r="C67" s="19"/>
       <c r="D67" s="19"/>
@@ -2160,7 +2204,7 @@
       <c r="H67" s="20"/>
     </row>
     <row r="68" ht="15.75" customHeight="1">
-      <c r="A68" s="21"/>
+      <c r="A68" s="22"/>
       <c r="B68" s="18"/>
       <c r="C68" s="19"/>
       <c r="D68" s="19"/>
@@ -2170,7 +2214,7 @@
       <c r="H68" s="20"/>
     </row>
     <row r="69" ht="15.75" customHeight="1">
-      <c r="A69" s="21"/>
+      <c r="A69" s="22"/>
       <c r="B69" s="18"/>
       <c r="C69" s="19"/>
       <c r="D69" s="19"/>
@@ -2180,7 +2224,7 @@
       <c r="H69" s="20"/>
     </row>
     <row r="70" ht="15.75" customHeight="1">
-      <c r="A70" s="21"/>
+      <c r="A70" s="22"/>
       <c r="B70" s="18"/>
       <c r="C70" s="19"/>
       <c r="D70" s="19"/>
@@ -2190,7 +2234,7 @@
       <c r="H70" s="20"/>
     </row>
     <row r="71" ht="15.75" customHeight="1">
-      <c r="A71" s="21"/>
+      <c r="A71" s="22"/>
       <c r="B71" s="18"/>
       <c r="C71" s="19"/>
       <c r="D71" s="19"/>
@@ -2200,7 +2244,7 @@
       <c r="H71" s="20"/>
     </row>
     <row r="72" ht="15.75" customHeight="1">
-      <c r="A72" s="21"/>
+      <c r="A72" s="22"/>
       <c r="B72" s="18"/>
       <c r="C72" s="19"/>
       <c r="D72" s="19"/>
@@ -2210,7 +2254,7 @@
       <c r="H72" s="20"/>
     </row>
     <row r="73" ht="15.75" customHeight="1">
-      <c r="A73" s="21"/>
+      <c r="A73" s="22"/>
       <c r="B73" s="18"/>
       <c r="C73" s="19"/>
       <c r="D73" s="19"/>
@@ -2220,7 +2264,7 @@
       <c r="H73" s="20"/>
     </row>
     <row r="74" ht="15.75" customHeight="1">
-      <c r="A74" s="21"/>
+      <c r="A74" s="22"/>
       <c r="B74" s="18"/>
       <c r="C74" s="19"/>
       <c r="D74" s="19"/>
@@ -2230,7 +2274,7 @@
       <c r="H74" s="20"/>
     </row>
     <row r="75" ht="15.75" customHeight="1">
-      <c r="A75" s="21"/>
+      <c r="A75" s="22"/>
       <c r="B75" s="18"/>
       <c r="C75" s="19"/>
       <c r="D75" s="19"/>
@@ -2240,7 +2284,7 @@
       <c r="H75" s="20"/>
     </row>
     <row r="76" ht="15.75" customHeight="1">
-      <c r="A76" s="21"/>
+      <c r="A76" s="22"/>
       <c r="B76" s="18"/>
       <c r="C76" s="19"/>
       <c r="D76" s="19"/>
@@ -2250,7 +2294,7 @@
       <c r="H76" s="20"/>
     </row>
     <row r="77" ht="15.75" customHeight="1">
-      <c r="A77" s="21"/>
+      <c r="A77" s="22"/>
       <c r="B77" s="18"/>
       <c r="C77" s="19"/>
       <c r="D77" s="19"/>
@@ -2260,7 +2304,7 @@
       <c r="H77" s="20"/>
     </row>
     <row r="78" ht="15.75" customHeight="1">
-      <c r="A78" s="21"/>
+      <c r="A78" s="22"/>
       <c r="B78" s="18"/>
       <c r="C78" s="19"/>
       <c r="D78" s="19"/>
@@ -2270,7 +2314,7 @@
       <c r="H78" s="20"/>
     </row>
     <row r="79" ht="15.75" customHeight="1">
-      <c r="A79" s="21"/>
+      <c r="A79" s="22"/>
       <c r="B79" s="18"/>
       <c r="C79" s="19"/>
       <c r="D79" s="19"/>
@@ -2280,7 +2324,7 @@
       <c r="H79" s="20"/>
     </row>
     <row r="80" ht="15.75" customHeight="1">
-      <c r="A80" s="21"/>
+      <c r="A80" s="22"/>
       <c r="B80" s="18"/>
       <c r="C80" s="19"/>
       <c r="D80" s="19"/>
@@ -2290,7 +2334,7 @@
       <c r="H80" s="20"/>
     </row>
     <row r="81" ht="15.75" customHeight="1">
-      <c r="A81" s="21"/>
+      <c r="A81" s="22"/>
       <c r="B81" s="18"/>
       <c r="C81" s="19"/>
       <c r="D81" s="19"/>
@@ -2300,7 +2344,7 @@
       <c r="H81" s="20"/>
     </row>
     <row r="82" ht="15.75" customHeight="1">
-      <c r="A82" s="21"/>
+      <c r="A82" s="22"/>
       <c r="B82" s="18"/>
       <c r="C82" s="19"/>
       <c r="D82" s="19"/>
@@ -2310,7 +2354,7 @@
       <c r="H82" s="20"/>
     </row>
     <row r="83" ht="15.75" customHeight="1">
-      <c r="A83" s="21"/>
+      <c r="A83" s="22"/>
       <c r="B83" s="18"/>
       <c r="C83" s="19"/>
       <c r="D83" s="19"/>
@@ -2320,7 +2364,7 @@
       <c r="H83" s="20"/>
     </row>
     <row r="84" ht="15.75" customHeight="1">
-      <c r="A84" s="21"/>
+      <c r="A84" s="22"/>
       <c r="B84" s="18"/>
       <c r="C84" s="19"/>
       <c r="D84" s="19"/>
@@ -2330,7 +2374,7 @@
       <c r="H84" s="20"/>
     </row>
     <row r="85" ht="15.75" customHeight="1">
-      <c r="A85" s="21"/>
+      <c r="A85" s="22"/>
       <c r="B85" s="18"/>
       <c r="C85" s="19"/>
       <c r="D85" s="19"/>
@@ -2340,7 +2384,7 @@
       <c r="H85" s="20"/>
     </row>
     <row r="86" ht="15.75" customHeight="1">
-      <c r="A86" s="21"/>
+      <c r="A86" s="22"/>
       <c r="B86" s="18"/>
       <c r="C86" s="19"/>
       <c r="D86" s="19"/>
@@ -2350,7 +2394,7 @@
       <c r="H86" s="20"/>
     </row>
     <row r="87" ht="15.75" customHeight="1">
-      <c r="A87" s="21"/>
+      <c r="A87" s="22"/>
       <c r="B87" s="18"/>
       <c r="C87" s="19"/>
       <c r="D87" s="19"/>
@@ -2360,7 +2404,7 @@
       <c r="H87" s="20"/>
     </row>
     <row r="88" ht="15.75" customHeight="1">
-      <c r="A88" s="21"/>
+      <c r="A88" s="22"/>
       <c r="B88" s="18"/>
       <c r="C88" s="19"/>
       <c r="D88" s="19"/>
@@ -2370,7 +2414,7 @@
       <c r="H88" s="20"/>
     </row>
     <row r="89" ht="15.75" customHeight="1">
-      <c r="A89" s="21"/>
+      <c r="A89" s="22"/>
       <c r="B89" s="18"/>
       <c r="C89" s="19"/>
       <c r="D89" s="19"/>
@@ -2380,7 +2424,7 @@
       <c r="H89" s="20"/>
     </row>
     <row r="90" ht="15.75" customHeight="1">
-      <c r="A90" s="21"/>
+      <c r="A90" s="22"/>
       <c r="B90" s="18"/>
       <c r="C90" s="19"/>
       <c r="D90" s="19"/>
@@ -2390,7 +2434,7 @@
       <c r="H90" s="20"/>
     </row>
     <row r="91" ht="15.75" customHeight="1">
-      <c r="A91" s="21"/>
+      <c r="A91" s="22"/>
       <c r="B91" s="18"/>
       <c r="C91" s="19"/>
       <c r="D91" s="19"/>
@@ -2400,7 +2444,7 @@
       <c r="H91" s="20"/>
     </row>
     <row r="92" ht="15.75" customHeight="1">
-      <c r="A92" s="21"/>
+      <c r="A92" s="22"/>
       <c r="B92" s="18"/>
       <c r="C92" s="19"/>
       <c r="D92" s="19"/>
@@ -2410,7 +2454,7 @@
       <c r="H92" s="20"/>
     </row>
     <row r="93" ht="15.75" customHeight="1">
-      <c r="A93" s="21"/>
+      <c r="A93" s="22"/>
       <c r="B93" s="18"/>
       <c r="C93" s="19"/>
       <c r="D93" s="19"/>
@@ -2420,7 +2464,7 @@
       <c r="H93" s="20"/>
     </row>
     <row r="94" ht="15.75" customHeight="1">
-      <c r="A94" s="21"/>
+      <c r="A94" s="22"/>
       <c r="B94" s="18"/>
       <c r="C94" s="19"/>
       <c r="D94" s="19"/>
@@ -2430,7 +2474,7 @@
       <c r="H94" s="20"/>
     </row>
     <row r="95" ht="15.75" customHeight="1">
-      <c r="A95" s="21"/>
+      <c r="A95" s="22"/>
       <c r="B95" s="18"/>
       <c r="C95" s="19"/>
       <c r="D95" s="19"/>
@@ -2440,7 +2484,7 @@
       <c r="H95" s="20"/>
     </row>
     <row r="96" ht="15.75" customHeight="1">
-      <c r="A96" s="21"/>
+      <c r="A96" s="22"/>
       <c r="B96" s="18"/>
       <c r="C96" s="19"/>
       <c r="D96" s="19"/>
@@ -2450,7 +2494,7 @@
       <c r="H96" s="20"/>
     </row>
     <row r="97" ht="15.75" customHeight="1">
-      <c r="A97" s="21"/>
+      <c r="A97" s="22"/>
       <c r="B97" s="18"/>
       <c r="C97" s="19"/>
       <c r="D97" s="19"/>
@@ -2460,7 +2504,7 @@
       <c r="H97" s="20"/>
     </row>
     <row r="98" ht="15.75" customHeight="1">
-      <c r="A98" s="21"/>
+      <c r="A98" s="22"/>
       <c r="B98" s="18"/>
       <c r="C98" s="19"/>
       <c r="D98" s="19"/>
@@ -2470,7 +2514,7 @@
       <c r="H98" s="20"/>
     </row>
     <row r="99" ht="15.75" customHeight="1">
-      <c r="A99" s="21"/>
+      <c r="A99" s="22"/>
       <c r="B99" s="18"/>
       <c r="C99" s="19"/>
       <c r="D99" s="19"/>
@@ -2480,7 +2524,7 @@
       <c r="H99" s="20"/>
     </row>
     <row r="100" ht="15.75" customHeight="1">
-      <c r="A100" s="21"/>
+      <c r="A100" s="22"/>
       <c r="B100" s="18"/>
       <c r="C100" s="19"/>
       <c r="D100" s="19"/>
@@ -2490,7 +2534,7 @@
       <c r="H100" s="20"/>
     </row>
     <row r="101" ht="15.75" customHeight="1">
-      <c r="A101" s="21"/>
+      <c r="A101" s="22"/>
       <c r="B101" s="18"/>
       <c r="C101" s="19"/>
       <c r="D101" s="19"/>
@@ -2500,7 +2544,7 @@
       <c r="H101" s="20"/>
     </row>
     <row r="102" ht="15.75" customHeight="1">
-      <c r="A102" s="21"/>
+      <c r="A102" s="22"/>
       <c r="B102" s="18"/>
       <c r="C102" s="19"/>
       <c r="D102" s="19"/>
@@ -2510,7 +2554,7 @@
       <c r="H102" s="20"/>
     </row>
     <row r="103" ht="15.75" customHeight="1">
-      <c r="A103" s="21"/>
+      <c r="A103" s="22"/>
       <c r="B103" s="18"/>
       <c r="C103" s="19"/>
       <c r="D103" s="19"/>
@@ -2520,7 +2564,7 @@
       <c r="H103" s="20"/>
     </row>
     <row r="104" ht="15.75" customHeight="1">
-      <c r="A104" s="21"/>
+      <c r="A104" s="22"/>
       <c r="B104" s="18"/>
       <c r="C104" s="19"/>
       <c r="D104" s="19"/>
@@ -2530,7 +2574,7 @@
       <c r="H104" s="20"/>
     </row>
     <row r="105" ht="15.75" customHeight="1">
-      <c r="A105" s="21"/>
+      <c r="A105" s="22"/>
       <c r="B105" s="18"/>
       <c r="C105" s="19"/>
       <c r="D105" s="19"/>
@@ -2540,8 +2584,8 @@
       <c r="H105" s="20"/>
     </row>
     <row r="106" ht="15.75" customHeight="1">
-      <c r="A106" s="21"/>
-      <c r="B106" s="21"/>
+      <c r="A106" s="22"/>
+      <c r="B106" s="22"/>
       <c r="C106" s="20"/>
       <c r="D106" s="20"/>
       <c r="E106" s="20"/>
@@ -2550,8 +2594,8 @@
       <c r="H106" s="20"/>
     </row>
     <row r="107" ht="15.75" customHeight="1">
-      <c r="A107" s="21"/>
-      <c r="B107" s="21"/>
+      <c r="A107" s="22"/>
+      <c r="B107" s="22"/>
       <c r="C107" s="20"/>
       <c r="D107" s="20"/>
       <c r="E107" s="20"/>
@@ -2560,8 +2604,8 @@
       <c r="H107" s="20"/>
     </row>
     <row r="108" ht="15.75" customHeight="1">
-      <c r="A108" s="21"/>
-      <c r="B108" s="21"/>
+      <c r="A108" s="22"/>
+      <c r="B108" s="22"/>
       <c r="C108" s="20"/>
       <c r="D108" s="20"/>
       <c r="E108" s="20"/>
@@ -2570,8 +2614,8 @@
       <c r="H108" s="20"/>
     </row>
     <row r="109" ht="15.75" customHeight="1">
-      <c r="A109" s="21"/>
-      <c r="B109" s="21"/>
+      <c r="A109" s="22"/>
+      <c r="B109" s="22"/>
       <c r="C109" s="4"/>
       <c r="D109" s="4"/>
       <c r="E109" s="4"/>
@@ -2580,8 +2624,8 @@
       <c r="H109" s="4"/>
     </row>
     <row r="110" ht="15.75" customHeight="1">
-      <c r="A110" s="21"/>
-      <c r="B110" s="21"/>
+      <c r="A110" s="22"/>
+      <c r="B110" s="22"/>
       <c r="C110" s="4"/>
       <c r="D110" s="4"/>
       <c r="E110" s="4"/>
@@ -2590,8 +2634,8 @@
       <c r="H110" s="4"/>
     </row>
     <row r="111" ht="15.75" customHeight="1">
-      <c r="A111" s="21"/>
-      <c r="B111" s="21"/>
+      <c r="A111" s="22"/>
+      <c r="B111" s="22"/>
       <c r="C111" s="4"/>
       <c r="D111" s="4"/>
       <c r="E111" s="4"/>
@@ -2600,8 +2644,8 @@
       <c r="H111" s="4"/>
     </row>
     <row r="112" ht="15.75" customHeight="1">
-      <c r="A112" s="21"/>
-      <c r="B112" s="21"/>
+      <c r="A112" s="22"/>
+      <c r="B112" s="22"/>
       <c r="C112" s="4"/>
       <c r="D112" s="4"/>
       <c r="E112" s="4"/>
@@ -2610,8 +2654,8 @@
       <c r="H112" s="4"/>
     </row>
     <row r="113" ht="15.75" customHeight="1">
-      <c r="A113" s="21"/>
-      <c r="B113" s="21"/>
+      <c r="A113" s="22"/>
+      <c r="B113" s="22"/>
       <c r="C113" s="4"/>
       <c r="D113" s="4"/>
       <c r="E113" s="4"/>
@@ -2620,8 +2664,8 @@
       <c r="H113" s="4"/>
     </row>
     <row r="114" ht="15.75" customHeight="1">
-      <c r="A114" s="21"/>
-      <c r="B114" s="21"/>
+      <c r="A114" s="22"/>
+      <c r="B114" s="22"/>
       <c r="C114" s="4"/>
       <c r="D114" s="4"/>
       <c r="E114" s="4"/>
@@ -2630,8 +2674,8 @@
       <c r="H114" s="4"/>
     </row>
     <row r="115" ht="15.75" customHeight="1">
-      <c r="A115" s="21"/>
-      <c r="B115" s="21"/>
+      <c r="A115" s="22"/>
+      <c r="B115" s="22"/>
       <c r="C115" s="4"/>
       <c r="D115" s="4"/>
       <c r="E115" s="4"/>
@@ -2640,8 +2684,8 @@
       <c r="H115" s="4"/>
     </row>
     <row r="116" ht="15.75" customHeight="1">
-      <c r="A116" s="21"/>
-      <c r="B116" s="21"/>
+      <c r="A116" s="22"/>
+      <c r="B116" s="22"/>
       <c r="C116" s="4"/>
       <c r="D116" s="4"/>
       <c r="E116" s="4"/>
@@ -2650,8 +2694,8 @@
       <c r="H116" s="4"/>
     </row>
     <row r="117" ht="15.75" customHeight="1">
-      <c r="A117" s="21"/>
-      <c r="B117" s="21"/>
+      <c r="A117" s="22"/>
+      <c r="B117" s="22"/>
       <c r="C117" s="4"/>
       <c r="D117" s="4"/>
       <c r="E117" s="4"/>
@@ -2660,8 +2704,8 @@
       <c r="H117" s="4"/>
     </row>
     <row r="118" ht="15.75" customHeight="1">
-      <c r="A118" s="21"/>
-      <c r="B118" s="21"/>
+      <c r="A118" s="22"/>
+      <c r="B118" s="22"/>
       <c r="C118" s="4"/>
       <c r="D118" s="4"/>
       <c r="E118" s="4"/>
@@ -2670,8 +2714,8 @@
       <c r="H118" s="4"/>
     </row>
     <row r="119" ht="15.75" customHeight="1">
-      <c r="A119" s="21"/>
-      <c r="B119" s="21"/>
+      <c r="A119" s="22"/>
+      <c r="B119" s="22"/>
       <c r="C119" s="4"/>
       <c r="D119" s="4"/>
       <c r="E119" s="4"/>
@@ -2680,8 +2724,8 @@
       <c r="H119" s="4"/>
     </row>
     <row r="120" ht="15.75" customHeight="1">
-      <c r="A120" s="21"/>
-      <c r="B120" s="21"/>
+      <c r="A120" s="22"/>
+      <c r="B120" s="22"/>
       <c r="C120" s="4"/>
       <c r="D120" s="4"/>
       <c r="E120" s="4"/>
@@ -2690,8 +2734,8 @@
       <c r="H120" s="4"/>
     </row>
     <row r="121" ht="15.75" customHeight="1">
-      <c r="A121" s="21"/>
-      <c r="B121" s="21"/>
+      <c r="A121" s="22"/>
+      <c r="B121" s="22"/>
       <c r="C121" s="4"/>
       <c r="D121" s="4"/>
       <c r="E121" s="4"/>
@@ -2700,8 +2744,8 @@
       <c r="H121" s="4"/>
     </row>
     <row r="122" ht="15.75" customHeight="1">
-      <c r="A122" s="21"/>
-      <c r="B122" s="21"/>
+      <c r="A122" s="22"/>
+      <c r="B122" s="22"/>
       <c r="C122" s="4"/>
       <c r="D122" s="4"/>
       <c r="E122" s="4"/>
@@ -2710,8 +2754,8 @@
       <c r="H122" s="4"/>
     </row>
     <row r="123" ht="15.75" customHeight="1">
-      <c r="A123" s="21"/>
-      <c r="B123" s="21"/>
+      <c r="A123" s="22"/>
+      <c r="B123" s="22"/>
       <c r="C123" s="4"/>
       <c r="D123" s="4"/>
       <c r="E123" s="4"/>
@@ -2720,8 +2764,8 @@
       <c r="H123" s="4"/>
     </row>
     <row r="124" ht="15.75" customHeight="1">
-      <c r="A124" s="21"/>
-      <c r="B124" s="21"/>
+      <c r="A124" s="22"/>
+      <c r="B124" s="22"/>
       <c r="C124" s="4"/>
       <c r="D124" s="4"/>
       <c r="E124" s="4"/>
@@ -2730,8 +2774,8 @@
       <c r="H124" s="4"/>
     </row>
     <row r="125" ht="15.75" customHeight="1">
-      <c r="A125" s="21"/>
-      <c r="B125" s="21"/>
+      <c r="A125" s="22"/>
+      <c r="B125" s="22"/>
       <c r="C125" s="4"/>
       <c r="D125" s="4"/>
       <c r="E125" s="4"/>
@@ -2740,8 +2784,8 @@
       <c r="H125" s="4"/>
     </row>
     <row r="126" ht="15.75" customHeight="1">
-      <c r="A126" s="21"/>
-      <c r="B126" s="21"/>
+      <c r="A126" s="22"/>
+      <c r="B126" s="22"/>
       <c r="C126" s="4"/>
       <c r="D126" s="4"/>
       <c r="E126" s="4"/>
@@ -2750,8 +2794,8 @@
       <c r="H126" s="4"/>
     </row>
     <row r="127" ht="15.75" customHeight="1">
-      <c r="A127" s="21"/>
-      <c r="B127" s="21"/>
+      <c r="A127" s="22"/>
+      <c r="B127" s="22"/>
       <c r="C127" s="4"/>
       <c r="D127" s="4"/>
       <c r="E127" s="4"/>
@@ -2760,8 +2804,8 @@
       <c r="H127" s="4"/>
     </row>
     <row r="128" ht="15.75" customHeight="1">
-      <c r="A128" s="21"/>
-      <c r="B128" s="21"/>
+      <c r="A128" s="22"/>
+      <c r="B128" s="22"/>
       <c r="C128" s="4"/>
       <c r="D128" s="4"/>
       <c r="E128" s="4"/>
@@ -2770,8 +2814,8 @@
       <c r="H128" s="4"/>
     </row>
     <row r="129" ht="15.75" customHeight="1">
-      <c r="A129" s="21"/>
-      <c r="B129" s="21"/>
+      <c r="A129" s="22"/>
+      <c r="B129" s="22"/>
       <c r="C129" s="4"/>
       <c r="D129" s="4"/>
       <c r="E129" s="4"/>
@@ -2780,8 +2824,8 @@
       <c r="H129" s="4"/>
     </row>
     <row r="130" ht="15.75" customHeight="1">
-      <c r="A130" s="21"/>
-      <c r="B130" s="21"/>
+      <c r="A130" s="22"/>
+      <c r="B130" s="22"/>
       <c r="C130" s="4"/>
       <c r="D130" s="4"/>
       <c r="E130" s="4"/>
@@ -2790,8 +2834,8 @@
       <c r="H130" s="4"/>
     </row>
     <row r="131" ht="15.75" customHeight="1">
-      <c r="A131" s="21"/>
-      <c r="B131" s="21"/>
+      <c r="A131" s="22"/>
+      <c r="B131" s="22"/>
       <c r="C131" s="4"/>
       <c r="D131" s="4"/>
       <c r="E131" s="4"/>
@@ -2800,8 +2844,8 @@
       <c r="H131" s="4"/>
     </row>
     <row r="132" ht="15.75" customHeight="1">
-      <c r="A132" s="21"/>
-      <c r="B132" s="21"/>
+      <c r="A132" s="22"/>
+      <c r="B132" s="22"/>
       <c r="C132" s="4"/>
       <c r="D132" s="4"/>
       <c r="E132" s="4"/>
@@ -2810,8 +2854,8 @@
       <c r="H132" s="4"/>
     </row>
     <row r="133" ht="15.75" customHeight="1">
-      <c r="A133" s="21"/>
-      <c r="B133" s="21"/>
+      <c r="A133" s="22"/>
+      <c r="B133" s="22"/>
       <c r="C133" s="4"/>
       <c r="D133" s="4"/>
       <c r="E133" s="4"/>
@@ -2820,8 +2864,8 @@
       <c r="H133" s="4"/>
     </row>
     <row r="134" ht="15.75" customHeight="1">
-      <c r="A134" s="21"/>
-      <c r="B134" s="21"/>
+      <c r="A134" s="22"/>
+      <c r="B134" s="22"/>
       <c r="C134" s="4"/>
       <c r="D134" s="4"/>
       <c r="E134" s="4"/>
@@ -2830,8 +2874,8 @@
       <c r="H134" s="4"/>
     </row>
     <row r="135" ht="15.75" customHeight="1">
-      <c r="A135" s="21"/>
-      <c r="B135" s="21"/>
+      <c r="A135" s="22"/>
+      <c r="B135" s="22"/>
       <c r="C135" s="4"/>
       <c r="D135" s="4"/>
       <c r="E135" s="4"/>
@@ -2840,8 +2884,8 @@
       <c r="H135" s="4"/>
     </row>
     <row r="136" ht="15.75" customHeight="1">
-      <c r="A136" s="21"/>
-      <c r="B136" s="21"/>
+      <c r="A136" s="22"/>
+      <c r="B136" s="22"/>
       <c r="C136" s="4"/>
       <c r="D136" s="4"/>
       <c r="E136" s="4"/>
@@ -2850,8 +2894,8 @@
       <c r="H136" s="4"/>
     </row>
     <row r="137" ht="15.75" customHeight="1">
-      <c r="A137" s="21"/>
-      <c r="B137" s="21"/>
+      <c r="A137" s="22"/>
+      <c r="B137" s="22"/>
       <c r="C137" s="4"/>
       <c r="D137" s="4"/>
       <c r="E137" s="4"/>
@@ -2860,8 +2904,8 @@
       <c r="H137" s="4"/>
     </row>
     <row r="138" ht="15.75" customHeight="1">
-      <c r="A138" s="21"/>
-      <c r="B138" s="21"/>
+      <c r="A138" s="22"/>
+      <c r="B138" s="22"/>
       <c r="C138" s="4"/>
       <c r="D138" s="4"/>
       <c r="E138" s="4"/>
@@ -2870,8 +2914,8 @@
       <c r="H138" s="4"/>
     </row>
     <row r="139" ht="15.75" customHeight="1">
-      <c r="A139" s="21"/>
-      <c r="B139" s="21"/>
+      <c r="A139" s="22"/>
+      <c r="B139" s="22"/>
       <c r="C139" s="4"/>
       <c r="D139" s="4"/>
       <c r="E139" s="4"/>
@@ -2880,8 +2924,8 @@
       <c r="H139" s="4"/>
     </row>
     <row r="140" ht="15.75" customHeight="1">
-      <c r="A140" s="21"/>
-      <c r="B140" s="21"/>
+      <c r="A140" s="22"/>
+      <c r="B140" s="22"/>
       <c r="C140" s="4"/>
       <c r="D140" s="4"/>
       <c r="E140" s="4"/>
@@ -2890,8 +2934,8 @@
       <c r="H140" s="4"/>
     </row>
     <row r="141" ht="15.75" customHeight="1">
-      <c r="A141" s="21"/>
-      <c r="B141" s="21"/>
+      <c r="A141" s="22"/>
+      <c r="B141" s="22"/>
       <c r="C141" s="4"/>
       <c r="D141" s="4"/>
       <c r="E141" s="4"/>
@@ -2900,8 +2944,8 @@
       <c r="H141" s="4"/>
     </row>
     <row r="142" ht="15.75" customHeight="1">
-      <c r="A142" s="21"/>
-      <c r="B142" s="21"/>
+      <c r="A142" s="22"/>
+      <c r="B142" s="22"/>
       <c r="C142" s="4"/>
       <c r="D142" s="4"/>
       <c r="E142" s="4"/>
@@ -2910,8 +2954,8 @@
       <c r="H142" s="4"/>
     </row>
     <row r="143" ht="15.75" customHeight="1">
-      <c r="A143" s="21"/>
-      <c r="B143" s="21"/>
+      <c r="A143" s="22"/>
+      <c r="B143" s="22"/>
       <c r="C143" s="4"/>
       <c r="D143" s="4"/>
       <c r="E143" s="4"/>
@@ -2920,8 +2964,8 @@
       <c r="H143" s="4"/>
     </row>
     <row r="144" ht="15.75" customHeight="1">
-      <c r="A144" s="21"/>
-      <c r="B144" s="21"/>
+      <c r="A144" s="22"/>
+      <c r="B144" s="22"/>
       <c r="C144" s="4"/>
       <c r="D144" s="4"/>
       <c r="E144" s="4"/>
@@ -2930,8 +2974,8 @@
       <c r="H144" s="4"/>
     </row>
     <row r="145" ht="15.75" customHeight="1">
-      <c r="A145" s="21"/>
-      <c r="B145" s="21"/>
+      <c r="A145" s="22"/>
+      <c r="B145" s="22"/>
       <c r="C145" s="4"/>
       <c r="D145" s="4"/>
       <c r="E145" s="4"/>
@@ -2940,8 +2984,8 @@
       <c r="H145" s="4"/>
     </row>
     <row r="146" ht="15.75" customHeight="1">
-      <c r="A146" s="21"/>
-      <c r="B146" s="21"/>
+      <c r="A146" s="22"/>
+      <c r="B146" s="22"/>
       <c r="C146" s="4"/>
       <c r="D146" s="4"/>
       <c r="E146" s="4"/>
@@ -2950,8 +2994,8 @@
       <c r="H146" s="4"/>
     </row>
     <row r="147" ht="15.75" customHeight="1">
-      <c r="A147" s="21"/>
-      <c r="B147" s="21"/>
+      <c r="A147" s="22"/>
+      <c r="B147" s="22"/>
       <c r="C147" s="4"/>
       <c r="D147" s="4"/>
       <c r="E147" s="4"/>
@@ -2960,8 +3004,8 @@
       <c r="H147" s="4"/>
     </row>
     <row r="148" ht="15.75" customHeight="1">
-      <c r="A148" s="21"/>
-      <c r="B148" s="21"/>
+      <c r="A148" s="22"/>
+      <c r="B148" s="22"/>
       <c r="C148" s="4"/>
       <c r="D148" s="4"/>
       <c r="E148" s="4"/>
@@ -2970,8 +3014,8 @@
       <c r="H148" s="4"/>
     </row>
     <row r="149" ht="15.75" customHeight="1">
-      <c r="A149" s="21"/>
-      <c r="B149" s="21"/>
+      <c r="A149" s="22"/>
+      <c r="B149" s="22"/>
       <c r="C149" s="4"/>
       <c r="D149" s="4"/>
       <c r="E149" s="4"/>
@@ -2980,8 +3024,8 @@
       <c r="H149" s="4"/>
     </row>
     <row r="150" ht="15.75" customHeight="1">
-      <c r="A150" s="21"/>
-      <c r="B150" s="21"/>
+      <c r="A150" s="22"/>
+      <c r="B150" s="22"/>
       <c r="C150" s="4"/>
       <c r="D150" s="4"/>
       <c r="E150" s="4"/>
@@ -2990,8 +3034,8 @@
       <c r="H150" s="4"/>
     </row>
     <row r="151" ht="15.75" customHeight="1">
-      <c r="A151" s="21"/>
-      <c r="B151" s="21"/>
+      <c r="A151" s="22"/>
+      <c r="B151" s="22"/>
       <c r="C151" s="4"/>
       <c r="D151" s="4"/>
       <c r="E151" s="4"/>
@@ -3000,8 +3044,8 @@
       <c r="H151" s="4"/>
     </row>
     <row r="152" ht="15.75" customHeight="1">
-      <c r="A152" s="21"/>
-      <c r="B152" s="21"/>
+      <c r="A152" s="22"/>
+      <c r="B152" s="22"/>
       <c r="C152" s="4"/>
       <c r="D152" s="4"/>
       <c r="E152" s="4"/>
@@ -3010,8 +3054,8 @@
       <c r="H152" s="4"/>
     </row>
     <row r="153" ht="15.75" customHeight="1">
-      <c r="A153" s="21"/>
-      <c r="B153" s="21"/>
+      <c r="A153" s="22"/>
+      <c r="B153" s="22"/>
       <c r="C153" s="4"/>
       <c r="D153" s="4"/>
       <c r="E153" s="4"/>
@@ -3020,8 +3064,8 @@
       <c r="H153" s="4"/>
     </row>
     <row r="154" ht="15.75" customHeight="1">
-      <c r="A154" s="21"/>
-      <c r="B154" s="21"/>
+      <c r="A154" s="22"/>
+      <c r="B154" s="22"/>
       <c r="C154" s="4"/>
       <c r="D154" s="4"/>
       <c r="E154" s="4"/>
@@ -3030,8 +3074,8 @@
       <c r="H154" s="4"/>
     </row>
     <row r="155" ht="15.75" customHeight="1">
-      <c r="A155" s="21"/>
-      <c r="B155" s="21"/>
+      <c r="A155" s="22"/>
+      <c r="B155" s="22"/>
       <c r="C155" s="4"/>
       <c r="D155" s="4"/>
       <c r="E155" s="4"/>
@@ -3040,8 +3084,8 @@
       <c r="H155" s="4"/>
     </row>
     <row r="156" ht="15.75" customHeight="1">
-      <c r="A156" s="21"/>
-      <c r="B156" s="21"/>
+      <c r="A156" s="22"/>
+      <c r="B156" s="22"/>
       <c r="C156" s="4"/>
       <c r="D156" s="4"/>
       <c r="E156" s="4"/>
@@ -3050,8 +3094,8 @@
       <c r="H156" s="4"/>
     </row>
     <row r="157" ht="15.75" customHeight="1">
-      <c r="A157" s="21"/>
-      <c r="B157" s="21"/>
+      <c r="A157" s="22"/>
+      <c r="B157" s="22"/>
       <c r="C157" s="4"/>
       <c r="D157" s="4"/>
       <c r="E157" s="4"/>
@@ -3060,8 +3104,8 @@
       <c r="H157" s="4"/>
     </row>
     <row r="158" ht="15.75" customHeight="1">
-      <c r="A158" s="21"/>
-      <c r="B158" s="21"/>
+      <c r="A158" s="22"/>
+      <c r="B158" s="22"/>
       <c r="C158" s="4"/>
       <c r="D158" s="4"/>
       <c r="E158" s="4"/>
@@ -3070,8 +3114,8 @@
       <c r="H158" s="4"/>
     </row>
     <row r="159" ht="15.75" customHeight="1">
-      <c r="A159" s="21"/>
-      <c r="B159" s="21"/>
+      <c r="A159" s="22"/>
+      <c r="B159" s="22"/>
       <c r="C159" s="4"/>
       <c r="D159" s="4"/>
       <c r="E159" s="4"/>
@@ -3080,8 +3124,8 @@
       <c r="H159" s="4"/>
     </row>
     <row r="160" ht="15.75" customHeight="1">
-      <c r="A160" s="21"/>
-      <c r="B160" s="21"/>
+      <c r="A160" s="22"/>
+      <c r="B160" s="22"/>
       <c r="C160" s="4"/>
       <c r="D160" s="4"/>
       <c r="E160" s="4"/>
@@ -3090,8 +3134,8 @@
       <c r="H160" s="4"/>
     </row>
     <row r="161" ht="15.75" customHeight="1">
-      <c r="A161" s="21"/>
-      <c r="B161" s="21"/>
+      <c r="A161" s="22"/>
+      <c r="B161" s="22"/>
       <c r="C161" s="4"/>
       <c r="D161" s="4"/>
       <c r="E161" s="4"/>
@@ -3100,8 +3144,8 @@
       <c r="H161" s="4"/>
     </row>
     <row r="162" ht="15.75" customHeight="1">
-      <c r="A162" s="21"/>
-      <c r="B162" s="21"/>
+      <c r="A162" s="22"/>
+      <c r="B162" s="22"/>
       <c r="C162" s="4"/>
       <c r="D162" s="4"/>
       <c r="E162" s="4"/>
@@ -3110,8 +3154,8 @@
       <c r="H162" s="4"/>
     </row>
     <row r="163" ht="15.75" customHeight="1">
-      <c r="A163" s="21"/>
-      <c r="B163" s="21"/>
+      <c r="A163" s="22"/>
+      <c r="B163" s="22"/>
       <c r="C163" s="4"/>
       <c r="D163" s="4"/>
       <c r="E163" s="4"/>
@@ -3120,8 +3164,8 @@
       <c r="H163" s="4"/>
     </row>
     <row r="164" ht="15.75" customHeight="1">
-      <c r="A164" s="21"/>
-      <c r="B164" s="21"/>
+      <c r="A164" s="22"/>
+      <c r="B164" s="22"/>
       <c r="C164" s="4"/>
       <c r="D164" s="4"/>
       <c r="E164" s="4"/>
@@ -3130,8 +3174,8 @@
       <c r="H164" s="4"/>
     </row>
     <row r="165" ht="15.75" customHeight="1">
-      <c r="A165" s="21"/>
-      <c r="B165" s="21"/>
+      <c r="A165" s="22"/>
+      <c r="B165" s="22"/>
       <c r="C165" s="4"/>
       <c r="D165" s="4"/>
       <c r="E165" s="4"/>
@@ -3140,8 +3184,8 @@
       <c r="H165" s="4"/>
     </row>
     <row r="166" ht="15.75" customHeight="1">
-      <c r="A166" s="21"/>
-      <c r="B166" s="21"/>
+      <c r="A166" s="22"/>
+      <c r="B166" s="22"/>
       <c r="C166" s="4"/>
       <c r="D166" s="4"/>
       <c r="E166" s="4"/>
@@ -3150,8 +3194,8 @@
       <c r="H166" s="4"/>
     </row>
     <row r="167" ht="15.75" customHeight="1">
-      <c r="A167" s="21"/>
-      <c r="B167" s="21"/>
+      <c r="A167" s="22"/>
+      <c r="B167" s="22"/>
       <c r="C167" s="4"/>
       <c r="D167" s="4"/>
       <c r="E167" s="4"/>
@@ -3160,8 +3204,8 @@
       <c r="H167" s="4"/>
     </row>
     <row r="168" ht="15.75" customHeight="1">
-      <c r="A168" s="21"/>
-      <c r="B168" s="21"/>
+      <c r="A168" s="22"/>
+      <c r="B168" s="22"/>
       <c r="C168" s="4"/>
       <c r="D168" s="4"/>
       <c r="E168" s="4"/>
@@ -3170,8 +3214,8 @@
       <c r="H168" s="4"/>
     </row>
     <row r="169" ht="15.75" customHeight="1">
-      <c r="A169" s="21"/>
-      <c r="B169" s="21"/>
+      <c r="A169" s="22"/>
+      <c r="B169" s="22"/>
       <c r="C169" s="4"/>
       <c r="D169" s="4"/>
       <c r="E169" s="4"/>
@@ -3180,8 +3224,8 @@
       <c r="H169" s="4"/>
     </row>
     <row r="170" ht="15.75" customHeight="1">
-      <c r="A170" s="21"/>
-      <c r="B170" s="21"/>
+      <c r="A170" s="22"/>
+      <c r="B170" s="22"/>
       <c r="C170" s="4"/>
       <c r="D170" s="4"/>
       <c r="E170" s="4"/>
@@ -3190,8 +3234,8 @@
       <c r="H170" s="4"/>
     </row>
     <row r="171" ht="15.75" customHeight="1">
-      <c r="A171" s="21"/>
-      <c r="B171" s="21"/>
+      <c r="A171" s="22"/>
+      <c r="B171" s="22"/>
       <c r="C171" s="4"/>
       <c r="D171" s="4"/>
       <c r="E171" s="4"/>
@@ -3200,8 +3244,8 @@
       <c r="H171" s="4"/>
     </row>
     <row r="172" ht="15.75" customHeight="1">
-      <c r="A172" s="21"/>
-      <c r="B172" s="21"/>
+      <c r="A172" s="22"/>
+      <c r="B172" s="22"/>
       <c r="C172" s="4"/>
       <c r="D172" s="4"/>
       <c r="E172" s="4"/>
@@ -3210,8 +3254,8 @@
       <c r="H172" s="4"/>
     </row>
     <row r="173" ht="15.75" customHeight="1">
-      <c r="A173" s="21"/>
-      <c r="B173" s="21"/>
+      <c r="A173" s="22"/>
+      <c r="B173" s="22"/>
       <c r="C173" s="4"/>
       <c r="D173" s="4"/>
       <c r="E173" s="4"/>
@@ -3220,8 +3264,8 @@
       <c r="H173" s="4"/>
     </row>
     <row r="174" ht="15.75" customHeight="1">
-      <c r="A174" s="21"/>
-      <c r="B174" s="21"/>
+      <c r="A174" s="22"/>
+      <c r="B174" s="22"/>
       <c r="C174" s="4"/>
       <c r="D174" s="4"/>
       <c r="E174" s="4"/>
@@ -3230,8 +3274,8 @@
       <c r="H174" s="4"/>
     </row>
     <row r="175" ht="15.75" customHeight="1">
-      <c r="A175" s="21"/>
-      <c r="B175" s="21"/>
+      <c r="A175" s="22"/>
+      <c r="B175" s="22"/>
       <c r="C175" s="4"/>
       <c r="D175" s="4"/>
       <c r="E175" s="4"/>
@@ -3240,8 +3284,8 @@
       <c r="H175" s="4"/>
     </row>
     <row r="176" ht="15.75" customHeight="1">
-      <c r="A176" s="21"/>
-      <c r="B176" s="21"/>
+      <c r="A176" s="22"/>
+      <c r="B176" s="22"/>
       <c r="C176" s="4"/>
       <c r="D176" s="4"/>
       <c r="E176" s="4"/>
@@ -3250,8 +3294,8 @@
       <c r="H176" s="4"/>
     </row>
     <row r="177" ht="15.75" customHeight="1">
-      <c r="A177" s="21"/>
-      <c r="B177" s="21"/>
+      <c r="A177" s="22"/>
+      <c r="B177" s="22"/>
       <c r="C177" s="4"/>
       <c r="D177" s="4"/>
       <c r="E177" s="4"/>
@@ -3260,8 +3304,8 @@
       <c r="H177" s="4"/>
     </row>
     <row r="178" ht="15.75" customHeight="1">
-      <c r="A178" s="21"/>
-      <c r="B178" s="21"/>
+      <c r="A178" s="22"/>
+      <c r="B178" s="22"/>
       <c r="C178" s="4"/>
       <c r="D178" s="4"/>
       <c r="E178" s="4"/>
@@ -3270,8 +3314,8 @@
       <c r="H178" s="4"/>
     </row>
     <row r="179" ht="15.75" customHeight="1">
-      <c r="A179" s="21"/>
-      <c r="B179" s="21"/>
+      <c r="A179" s="22"/>
+      <c r="B179" s="22"/>
       <c r="C179" s="4"/>
       <c r="D179" s="4"/>
       <c r="E179" s="4"/>
@@ -3280,8 +3324,8 @@
       <c r="H179" s="4"/>
     </row>
     <row r="180" ht="15.75" customHeight="1">
-      <c r="A180" s="21"/>
-      <c r="B180" s="21"/>
+      <c r="A180" s="22"/>
+      <c r="B180" s="22"/>
       <c r="C180" s="4"/>
       <c r="D180" s="4"/>
       <c r="E180" s="4"/>
@@ -3290,8 +3334,8 @@
       <c r="H180" s="4"/>
     </row>
     <row r="181" ht="15.75" customHeight="1">
-      <c r="A181" s="21"/>
-      <c r="B181" s="21"/>
+      <c r="A181" s="22"/>
+      <c r="B181" s="22"/>
       <c r="C181" s="4"/>
       <c r="D181" s="4"/>
       <c r="E181" s="4"/>
@@ -3300,8 +3344,8 @@
       <c r="H181" s="4"/>
     </row>
     <row r="182" ht="15.75" customHeight="1">
-      <c r="A182" s="21"/>
-      <c r="B182" s="21"/>
+      <c r="A182" s="22"/>
+      <c r="B182" s="22"/>
       <c r="C182" s="4"/>
       <c r="D182" s="4"/>
       <c r="E182" s="4"/>
@@ -3310,8 +3354,8 @@
       <c r="H182" s="4"/>
     </row>
     <row r="183" ht="15.75" customHeight="1">
-      <c r="A183" s="21"/>
-      <c r="B183" s="21"/>
+      <c r="A183" s="22"/>
+      <c r="B183" s="22"/>
       <c r="C183" s="4"/>
       <c r="D183" s="4"/>
       <c r="E183" s="4"/>
@@ -3320,8 +3364,8 @@
       <c r="H183" s="4"/>
     </row>
     <row r="184" ht="15.75" customHeight="1">
-      <c r="A184" s="21"/>
-      <c r="B184" s="21"/>
+      <c r="A184" s="22"/>
+      <c r="B184" s="22"/>
       <c r="C184" s="4"/>
       <c r="D184" s="4"/>
       <c r="E184" s="4"/>
@@ -3330,8 +3374,8 @@
       <c r="H184" s="4"/>
     </row>
     <row r="185" ht="15.75" customHeight="1">
-      <c r="A185" s="21"/>
-      <c r="B185" s="21"/>
+      <c r="A185" s="22"/>
+      <c r="B185" s="22"/>
       <c r="C185" s="4"/>
       <c r="D185" s="4"/>
       <c r="E185" s="4"/>
@@ -3340,8 +3384,8 @@
       <c r="H185" s="4"/>
     </row>
     <row r="186" ht="15.75" customHeight="1">
-      <c r="A186" s="21"/>
-      <c r="B186" s="21"/>
+      <c r="A186" s="22"/>
+      <c r="B186" s="22"/>
       <c r="C186" s="4"/>
       <c r="D186" s="4"/>
       <c r="E186" s="4"/>
@@ -3350,8 +3394,8 @@
       <c r="H186" s="4"/>
     </row>
     <row r="187" ht="15.75" customHeight="1">
-      <c r="A187" s="21"/>
-      <c r="B187" s="21"/>
+      <c r="A187" s="22"/>
+      <c r="B187" s="22"/>
       <c r="C187" s="4"/>
       <c r="D187" s="4"/>
       <c r="E187" s="4"/>
@@ -3360,8 +3404,8 @@
       <c r="H187" s="4"/>
     </row>
     <row r="188" ht="15.75" customHeight="1">
-      <c r="A188" s="21"/>
-      <c r="B188" s="21"/>
+      <c r="A188" s="22"/>
+      <c r="B188" s="22"/>
       <c r="C188" s="4"/>
       <c r="D188" s="4"/>
       <c r="E188" s="4"/>
@@ -3370,8 +3414,8 @@
       <c r="H188" s="4"/>
     </row>
     <row r="189" ht="15.75" customHeight="1">
-      <c r="A189" s="21"/>
-      <c r="B189" s="21"/>
+      <c r="A189" s="22"/>
+      <c r="B189" s="22"/>
       <c r="C189" s="4"/>
       <c r="D189" s="4"/>
       <c r="E189" s="4"/>
@@ -3380,8 +3424,8 @@
       <c r="H189" s="4"/>
     </row>
     <row r="190" ht="15.75" customHeight="1">
-      <c r="A190" s="21"/>
-      <c r="B190" s="21"/>
+      <c r="A190" s="22"/>
+      <c r="B190" s="22"/>
       <c r="C190" s="4"/>
       <c r="D190" s="4"/>
       <c r="E190" s="4"/>
@@ -3390,8 +3434,8 @@
       <c r="H190" s="4"/>
     </row>
     <row r="191" ht="15.75" customHeight="1">
-      <c r="A191" s="21"/>
-      <c r="B191" s="21"/>
+      <c r="A191" s="22"/>
+      <c r="B191" s="22"/>
       <c r="C191" s="4"/>
       <c r="D191" s="4"/>
       <c r="E191" s="4"/>
@@ -3400,8 +3444,8 @@
       <c r="H191" s="4"/>
     </row>
     <row r="192" ht="15.75" customHeight="1">
-      <c r="A192" s="21"/>
-      <c r="B192" s="21"/>
+      <c r="A192" s="22"/>
+      <c r="B192" s="22"/>
       <c r="C192" s="4"/>
       <c r="D192" s="4"/>
       <c r="E192" s="4"/>
@@ -3410,8 +3454,8 @@
       <c r="H192" s="4"/>
     </row>
     <row r="193" ht="15.75" customHeight="1">
-      <c r="A193" s="21"/>
-      <c r="B193" s="21"/>
+      <c r="A193" s="22"/>
+      <c r="B193" s="22"/>
       <c r="C193" s="4"/>
       <c r="D193" s="4"/>
       <c r="E193" s="4"/>
@@ -3420,8 +3464,8 @@
       <c r="H193" s="4"/>
     </row>
     <row r="194" ht="15.75" customHeight="1">
-      <c r="A194" s="21"/>
-      <c r="B194" s="21"/>
+      <c r="A194" s="22"/>
+      <c r="B194" s="22"/>
       <c r="C194" s="4"/>
       <c r="D194" s="4"/>
       <c r="E194" s="4"/>
@@ -3430,8 +3474,8 @@
       <c r="H194" s="4"/>
     </row>
     <row r="195" ht="15.75" customHeight="1">
-      <c r="A195" s="21"/>
-      <c r="B195" s="21"/>
+      <c r="A195" s="22"/>
+      <c r="B195" s="22"/>
       <c r="C195" s="4"/>
       <c r="D195" s="4"/>
       <c r="E195" s="4"/>
@@ -3440,8 +3484,8 @@
       <c r="H195" s="4"/>
     </row>
     <row r="196" ht="15.75" customHeight="1">
-      <c r="A196" s="21"/>
-      <c r="B196" s="21"/>
+      <c r="A196" s="22"/>
+      <c r="B196" s="22"/>
       <c r="C196" s="4"/>
       <c r="D196" s="4"/>
       <c r="E196" s="4"/>
@@ -3450,8 +3494,8 @@
       <c r="H196" s="4"/>
     </row>
     <row r="197" ht="15.75" customHeight="1">
-      <c r="A197" s="21"/>
-      <c r="B197" s="21"/>
+      <c r="A197" s="22"/>
+      <c r="B197" s="22"/>
       <c r="C197" s="4"/>
       <c r="D197" s="4"/>
       <c r="E197" s="4"/>
@@ -3460,8 +3504,8 @@
       <c r="H197" s="4"/>
     </row>
     <row r="198" ht="15.75" customHeight="1">
-      <c r="A198" s="21"/>
-      <c r="B198" s="21"/>
+      <c r="A198" s="22"/>
+      <c r="B198" s="22"/>
       <c r="C198" s="4"/>
       <c r="D198" s="4"/>
       <c r="E198" s="4"/>
@@ -3470,8 +3514,8 @@
       <c r="H198" s="4"/>
     </row>
     <row r="199" ht="15.75" customHeight="1">
-      <c r="A199" s="21"/>
-      <c r="B199" s="21"/>
+      <c r="A199" s="22"/>
+      <c r="B199" s="22"/>
       <c r="C199" s="4"/>
       <c r="D199" s="4"/>
       <c r="E199" s="4"/>
@@ -3480,8 +3524,8 @@
       <c r="H199" s="4"/>
     </row>
     <row r="200" ht="15.75" customHeight="1">
-      <c r="A200" s="21"/>
-      <c r="B200" s="21"/>
+      <c r="A200" s="22"/>
+      <c r="B200" s="22"/>
       <c r="C200" s="4"/>
       <c r="D200" s="4"/>
       <c r="E200" s="4"/>
@@ -3490,8 +3534,8 @@
       <c r="H200" s="4"/>
     </row>
     <row r="201" ht="15.75" customHeight="1">
-      <c r="A201" s="21"/>
-      <c r="B201" s="21"/>
+      <c r="A201" s="22"/>
+      <c r="B201" s="22"/>
       <c r="C201" s="4"/>
       <c r="D201" s="4"/>
       <c r="E201" s="4"/>
@@ -3500,8 +3544,8 @@
       <c r="H201" s="4"/>
     </row>
     <row r="202" ht="15.75" customHeight="1">
-      <c r="A202" s="21"/>
-      <c r="B202" s="21"/>
+      <c r="A202" s="22"/>
+      <c r="B202" s="22"/>
       <c r="C202" s="4"/>
       <c r="D202" s="4"/>
       <c r="E202" s="4"/>
@@ -3510,8 +3554,8 @@
       <c r="H202" s="4"/>
     </row>
     <row r="203" ht="15.75" customHeight="1">
-      <c r="A203" s="21"/>
-      <c r="B203" s="21"/>
+      <c r="A203" s="22"/>
+      <c r="B203" s="22"/>
       <c r="C203" s="4"/>
       <c r="D203" s="4"/>
       <c r="E203" s="4"/>
@@ -3520,8 +3564,8 @@
       <c r="H203" s="4"/>
     </row>
     <row r="204" ht="15.75" customHeight="1">
-      <c r="A204" s="21"/>
-      <c r="B204" s="21"/>
+      <c r="A204" s="22"/>
+      <c r="B204" s="22"/>
       <c r="C204" s="4"/>
       <c r="D204" s="4"/>
       <c r="E204" s="4"/>
@@ -3530,8 +3574,8 @@
       <c r="H204" s="4"/>
     </row>
     <row r="205" ht="15.75" customHeight="1">
-      <c r="A205" s="21"/>
-      <c r="B205" s="21"/>
+      <c r="A205" s="22"/>
+      <c r="B205" s="22"/>
       <c r="C205" s="4"/>
       <c r="D205" s="4"/>
       <c r="E205" s="4"/>
@@ -3540,8 +3584,8 @@
       <c r="H205" s="4"/>
     </row>
     <row r="206" ht="15.75" customHeight="1">
-      <c r="A206" s="21"/>
-      <c r="B206" s="21"/>
+      <c r="A206" s="22"/>
+      <c r="B206" s="22"/>
       <c r="C206" s="4"/>
       <c r="D206" s="4"/>
       <c r="E206" s="4"/>
@@ -3550,8 +3594,8 @@
       <c r="H206" s="4"/>
     </row>
     <row r="207" ht="15.75" customHeight="1">
-      <c r="A207" s="21"/>
-      <c r="B207" s="21"/>
+      <c r="A207" s="22"/>
+      <c r="B207" s="22"/>
       <c r="C207" s="4"/>
       <c r="D207" s="4"/>
       <c r="E207" s="4"/>
@@ -3560,8 +3604,8 @@
       <c r="H207" s="4"/>
     </row>
     <row r="208" ht="15.75" customHeight="1">
-      <c r="A208" s="21"/>
-      <c r="B208" s="21"/>
+      <c r="A208" s="22"/>
+      <c r="B208" s="22"/>
       <c r="C208" s="4"/>
       <c r="D208" s="4"/>
       <c r="E208" s="4"/>
@@ -3570,8 +3614,8 @@
       <c r="H208" s="4"/>
     </row>
     <row r="209" ht="15.75" customHeight="1">
-      <c r="A209" s="21"/>
-      <c r="B209" s="21"/>
+      <c r="A209" s="22"/>
+      <c r="B209" s="22"/>
       <c r="C209" s="4"/>
       <c r="D209" s="4"/>
       <c r="E209" s="4"/>
@@ -3580,8 +3624,8 @@
       <c r="H209" s="4"/>
     </row>
     <row r="210" ht="15.75" customHeight="1">
-      <c r="A210" s="21"/>
-      <c r="B210" s="21"/>
+      <c r="A210" s="22"/>
+      <c r="B210" s="22"/>
       <c r="C210" s="4"/>
       <c r="D210" s="4"/>
       <c r="E210" s="4"/>
@@ -3590,8 +3634,8 @@
       <c r="H210" s="4"/>
     </row>
     <row r="211" ht="15.75" customHeight="1">
-      <c r="A211" s="21"/>
-      <c r="B211" s="21"/>
+      <c r="A211" s="22"/>
+      <c r="B211" s="22"/>
       <c r="C211" s="4"/>
       <c r="D211" s="4"/>
       <c r="E211" s="4"/>
@@ -3600,8 +3644,8 @@
       <c r="H211" s="4"/>
     </row>
     <row r="212" ht="15.75" customHeight="1">
-      <c r="A212" s="21"/>
-      <c r="B212" s="21"/>
+      <c r="A212" s="22"/>
+      <c r="B212" s="22"/>
       <c r="C212" s="4"/>
       <c r="D212" s="4"/>
       <c r="E212" s="4"/>
@@ -3610,8 +3654,8 @@
       <c r="H212" s="4"/>
     </row>
     <row r="213" ht="15.75" customHeight="1">
-      <c r="A213" s="21"/>
-      <c r="B213" s="21"/>
+      <c r="A213" s="22"/>
+      <c r="B213" s="22"/>
       <c r="C213" s="4"/>
       <c r="D213" s="4"/>
       <c r="E213" s="4"/>
@@ -3620,8 +3664,8 @@
       <c r="H213" s="4"/>
     </row>
     <row r="214" ht="15.75" customHeight="1">
-      <c r="A214" s="21"/>
-      <c r="B214" s="21"/>
+      <c r="A214" s="22"/>
+      <c r="B214" s="22"/>
       <c r="C214" s="4"/>
       <c r="D214" s="4"/>
       <c r="E214" s="4"/>
@@ -3630,8 +3674,8 @@
       <c r="H214" s="4"/>
     </row>
     <row r="215" ht="15.75" customHeight="1">
-      <c r="A215" s="21"/>
-      <c r="B215" s="21"/>
+      <c r="A215" s="22"/>
+      <c r="B215" s="22"/>
       <c r="C215" s="4"/>
       <c r="D215" s="4"/>
       <c r="E215" s="4"/>
@@ -3640,8 +3684,8 @@
       <c r="H215" s="4"/>
     </row>
     <row r="216" ht="15.75" customHeight="1">
-      <c r="A216" s="21"/>
-      <c r="B216" s="21"/>
+      <c r="A216" s="22"/>
+      <c r="B216" s="22"/>
       <c r="C216" s="4"/>
       <c r="D216" s="4"/>
       <c r="E216" s="4"/>
@@ -3650,8 +3694,8 @@
       <c r="H216" s="4"/>
     </row>
     <row r="217" ht="15.75" customHeight="1">
-      <c r="A217" s="21"/>
-      <c r="B217" s="21"/>
+      <c r="A217" s="22"/>
+      <c r="B217" s="22"/>
       <c r="C217" s="4"/>
       <c r="D217" s="4"/>
       <c r="E217" s="4"/>
@@ -3660,8 +3704,8 @@
       <c r="H217" s="4"/>
     </row>
     <row r="218" ht="15.75" customHeight="1">
-      <c r="A218" s="21"/>
-      <c r="B218" s="21"/>
+      <c r="A218" s="22"/>
+      <c r="B218" s="22"/>
       <c r="C218" s="4"/>
       <c r="D218" s="4"/>
       <c r="E218" s="4"/>
@@ -3670,8 +3714,8 @@
       <c r="H218" s="4"/>
     </row>
     <row r="219" ht="15.75" customHeight="1">
-      <c r="A219" s="21"/>
-      <c r="B219" s="21"/>
+      <c r="A219" s="22"/>
+      <c r="B219" s="22"/>
       <c r="C219" s="4"/>
       <c r="D219" s="4"/>
       <c r="E219" s="4"/>
@@ -3680,8 +3724,8 @@
       <c r="H219" s="4"/>
     </row>
     <row r="220" ht="15.75" customHeight="1">
-      <c r="A220" s="21"/>
-      <c r="B220" s="21"/>
+      <c r="A220" s="22"/>
+      <c r="B220" s="22"/>
       <c r="C220" s="4"/>
       <c r="D220" s="4"/>
       <c r="E220" s="4"/>
@@ -3690,7 +3734,7 @@
       <c r="H220" s="4"/>
     </row>
     <row r="221" ht="13.5" customHeight="1">
-      <c r="A221" s="21"/>
+      <c r="A221" s="22"/>
       <c r="B221" s="4"/>
       <c r="C221" s="4"/>
       <c r="D221" s="4"/>
@@ -3700,7 +3744,7 @@
       <c r="H221" s="4"/>
     </row>
     <row r="222" ht="13.5" customHeight="1">
-      <c r="A222" s="21"/>
+      <c r="A222" s="22"/>
       <c r="B222" s="4"/>
       <c r="C222" s="4"/>
       <c r="D222" s="4"/>
@@ -3710,7 +3754,7 @@
       <c r="H222" s="4"/>
     </row>
     <row r="223" ht="13.5" customHeight="1">
-      <c r="A223" s="21"/>
+      <c r="A223" s="22"/>
       <c r="B223" s="4"/>
       <c r="C223" s="4"/>
       <c r="D223" s="4"/>
@@ -3720,7 +3764,7 @@
       <c r="H223" s="4"/>
     </row>
     <row r="224" ht="13.5" customHeight="1">
-      <c r="A224" s="21"/>
+      <c r="A224" s="22"/>
       <c r="B224" s="4"/>
       <c r="C224" s="4"/>
       <c r="D224" s="4"/>
@@ -3730,7 +3774,7 @@
       <c r="H224" s="4"/>
     </row>
     <row r="225" ht="13.5" customHeight="1">
-      <c r="A225" s="21"/>
+      <c r="A225" s="22"/>
       <c r="B225" s="4"/>
       <c r="C225" s="4"/>
       <c r="D225" s="4"/>
@@ -3740,7 +3784,7 @@
       <c r="H225" s="4"/>
     </row>
     <row r="226" ht="13.5" customHeight="1">
-      <c r="A226" s="21"/>
+      <c r="A226" s="22"/>
       <c r="B226" s="4"/>
       <c r="C226" s="4"/>
       <c r="D226" s="4"/>
@@ -3750,7 +3794,7 @@
       <c r="H226" s="4"/>
     </row>
     <row r="227" ht="13.5" customHeight="1">
-      <c r="A227" s="21"/>
+      <c r="A227" s="22"/>
       <c r="B227" s="4"/>
       <c r="C227" s="4"/>
       <c r="D227" s="4"/>
@@ -3760,7 +3804,7 @@
       <c r="H227" s="4"/>
     </row>
     <row r="228" ht="13.5" customHeight="1">
-      <c r="A228" s="21"/>
+      <c r="A228" s="22"/>
       <c r="B228" s="4"/>
       <c r="C228" s="4"/>
       <c r="D228" s="4"/>
@@ -3770,7 +3814,7 @@
       <c r="H228" s="4"/>
     </row>
     <row r="229" ht="13.5" customHeight="1">
-      <c r="A229" s="21"/>
+      <c r="A229" s="22"/>
       <c r="B229" s="4"/>
       <c r="C229" s="4"/>
       <c r="D229" s="4"/>
@@ -3780,7 +3824,7 @@
       <c r="H229" s="4"/>
     </row>
     <row r="230" ht="13.5" customHeight="1">
-      <c r="A230" s="21"/>
+      <c r="A230" s="22"/>
       <c r="B230" s="4"/>
       <c r="C230" s="4"/>
       <c r="D230" s="4"/>
@@ -3790,7 +3834,7 @@
       <c r="H230" s="4"/>
     </row>
     <row r="231" ht="13.5" customHeight="1">
-      <c r="A231" s="21"/>
+      <c r="A231" s="22"/>
       <c r="B231" s="4"/>
       <c r="C231" s="4"/>
       <c r="D231" s="4"/>
@@ -3800,7 +3844,7 @@
       <c r="H231" s="4"/>
     </row>
     <row r="232" ht="13.5" customHeight="1">
-      <c r="A232" s="21"/>
+      <c r="A232" s="22"/>
       <c r="B232" s="4"/>
       <c r="C232" s="4"/>
       <c r="D232" s="4"/>
@@ -3810,7 +3854,7 @@
       <c r="H232" s="4"/>
     </row>
     <row r="233" ht="13.5" customHeight="1">
-      <c r="A233" s="21"/>
+      <c r="A233" s="22"/>
       <c r="B233" s="4"/>
       <c r="C233" s="4"/>
       <c r="D233" s="4"/>
@@ -3820,7 +3864,7 @@
       <c r="H233" s="4"/>
     </row>
     <row r="234" ht="13.5" customHeight="1">
-      <c r="A234" s="21"/>
+      <c r="A234" s="22"/>
       <c r="B234" s="4"/>
       <c r="C234" s="4"/>
       <c r="D234" s="4"/>
@@ -3830,7 +3874,7 @@
       <c r="H234" s="4"/>
     </row>
     <row r="235" ht="13.5" customHeight="1">
-      <c r="A235" s="21"/>
+      <c r="A235" s="22"/>
       <c r="B235" s="4"/>
       <c r="C235" s="4"/>
       <c r="D235" s="4"/>
@@ -3840,7 +3884,7 @@
       <c r="H235" s="4"/>
     </row>
     <row r="236" ht="13.5" customHeight="1">
-      <c r="A236" s="21"/>
+      <c r="A236" s="22"/>
       <c r="B236" s="4"/>
       <c r="C236" s="4"/>
       <c r="D236" s="4"/>
@@ -3850,7 +3894,7 @@
       <c r="H236" s="4"/>
     </row>
     <row r="237" ht="13.5" customHeight="1">
-      <c r="A237" s="21"/>
+      <c r="A237" s="22"/>
       <c r="B237" s="4"/>
       <c r="C237" s="4"/>
       <c r="D237" s="4"/>
@@ -3860,7 +3904,7 @@
       <c r="H237" s="4"/>
     </row>
     <row r="238" ht="13.5" customHeight="1">
-      <c r="A238" s="21"/>
+      <c r="A238" s="22"/>
       <c r="B238" s="4"/>
       <c r="C238" s="4"/>
       <c r="D238" s="4"/>
@@ -3870,7 +3914,7 @@
       <c r="H238" s="4"/>
     </row>
     <row r="239" ht="13.5" customHeight="1">
-      <c r="A239" s="21"/>
+      <c r="A239" s="22"/>
       <c r="B239" s="4"/>
       <c r="C239" s="4"/>
       <c r="D239" s="4"/>
@@ -3880,7 +3924,7 @@
       <c r="H239" s="4"/>
     </row>
     <row r="240" ht="13.5" customHeight="1">
-      <c r="A240" s="21"/>
+      <c r="A240" s="22"/>
       <c r="B240" s="4"/>
       <c r="C240" s="4"/>
       <c r="D240" s="4"/>
@@ -3890,7 +3934,7 @@
       <c r="H240" s="4"/>
     </row>
     <row r="241" ht="13.5" customHeight="1">
-      <c r="A241" s="21"/>
+      <c r="A241" s="22"/>
       <c r="B241" s="4"/>
       <c r="C241" s="4"/>
       <c r="D241" s="4"/>
@@ -3900,7 +3944,7 @@
       <c r="H241" s="4"/>
     </row>
     <row r="242" ht="13.5" customHeight="1">
-      <c r="A242" s="21"/>
+      <c r="A242" s="22"/>
       <c r="B242" s="4"/>
       <c r="C242" s="4"/>
       <c r="D242" s="4"/>
@@ -3910,7 +3954,7 @@
       <c r="H242" s="4"/>
     </row>
     <row r="243" ht="13.5" customHeight="1">
-      <c r="A243" s="21"/>
+      <c r="A243" s="22"/>
       <c r="B243" s="4"/>
       <c r="C243" s="4"/>
       <c r="D243" s="4"/>
@@ -3920,7 +3964,7 @@
       <c r="H243" s="4"/>
     </row>
     <row r="244" ht="13.5" customHeight="1">
-      <c r="A244" s="21"/>
+      <c r="A244" s="22"/>
       <c r="B244" s="4"/>
       <c r="C244" s="4"/>
       <c r="D244" s="4"/>
@@ -3930,7 +3974,7 @@
       <c r="H244" s="4"/>
     </row>
     <row r="245" ht="13.5" customHeight="1">
-      <c r="A245" s="21"/>
+      <c r="A245" s="22"/>
       <c r="B245" s="4"/>
       <c r="C245" s="4"/>
       <c r="D245" s="4"/>
@@ -3940,7 +3984,7 @@
       <c r="H245" s="4"/>
     </row>
     <row r="246" ht="13.5" customHeight="1">
-      <c r="A246" s="21"/>
+      <c r="A246" s="22"/>
       <c r="B246" s="4"/>
       <c r="C246" s="4"/>
       <c r="D246" s="4"/>
@@ -3950,7 +3994,7 @@
       <c r="H246" s="4"/>
     </row>
     <row r="247" ht="13.5" customHeight="1">
-      <c r="A247" s="21"/>
+      <c r="A247" s="22"/>
       <c r="B247" s="4"/>
       <c r="C247" s="4"/>
       <c r="D247" s="4"/>
@@ -3960,7 +4004,7 @@
       <c r="H247" s="4"/>
     </row>
     <row r="248" ht="13.5" customHeight="1">
-      <c r="A248" s="21"/>
+      <c r="A248" s="22"/>
       <c r="B248" s="4"/>
       <c r="C248" s="4"/>
       <c r="D248" s="4"/>
@@ -3970,7 +4014,7 @@
       <c r="H248" s="4"/>
     </row>
     <row r="249" ht="13.5" customHeight="1">
-      <c r="A249" s="21"/>
+      <c r="A249" s="22"/>
       <c r="B249" s="4"/>
       <c r="C249" s="4"/>
       <c r="D249" s="4"/>
@@ -3980,7 +4024,7 @@
       <c r="H249" s="4"/>
     </row>
     <row r="250" ht="13.5" customHeight="1">
-      <c r="A250" s="21"/>
+      <c r="A250" s="22"/>
       <c r="B250" s="4"/>
       <c r="C250" s="4"/>
       <c r="D250" s="4"/>
@@ -3990,7 +4034,7 @@
       <c r="H250" s="4"/>
     </row>
     <row r="251" ht="13.5" customHeight="1">
-      <c r="A251" s="21"/>
+      <c r="A251" s="22"/>
       <c r="B251" s="4"/>
       <c r="C251" s="4"/>
       <c r="D251" s="4"/>
@@ -4000,7 +4044,7 @@
       <c r="H251" s="4"/>
     </row>
     <row r="252" ht="13.5" customHeight="1">
-      <c r="A252" s="21"/>
+      <c r="A252" s="22"/>
       <c r="B252" s="4"/>
       <c r="C252" s="4"/>
       <c r="D252" s="4"/>
@@ -4010,7 +4054,7 @@
       <c r="H252" s="4"/>
     </row>
     <row r="253" ht="13.5" customHeight="1">
-      <c r="A253" s="21"/>
+      <c r="A253" s="22"/>
       <c r="B253" s="4"/>
       <c r="C253" s="4"/>
       <c r="D253" s="4"/>
@@ -4020,7 +4064,7 @@
       <c r="H253" s="4"/>
     </row>
     <row r="254" ht="13.5" customHeight="1">
-      <c r="A254" s="21"/>
+      <c r="A254" s="22"/>
       <c r="B254" s="4"/>
       <c r="C254" s="4"/>
       <c r="D254" s="4"/>
@@ -4030,7 +4074,7 @@
       <c r="H254" s="4"/>
     </row>
     <row r="255" ht="13.5" customHeight="1">
-      <c r="A255" s="21"/>
+      <c r="A255" s="22"/>
       <c r="B255" s="4"/>
       <c r="C255" s="4"/>
       <c r="D255" s="4"/>
@@ -4040,7 +4084,7 @@
       <c r="H255" s="4"/>
     </row>
     <row r="256" ht="13.5" customHeight="1">
-      <c r="A256" s="21"/>
+      <c r="A256" s="22"/>
       <c r="B256" s="4"/>
       <c r="C256" s="4"/>
       <c r="D256" s="4"/>
@@ -4050,7 +4094,7 @@
       <c r="H256" s="4"/>
     </row>
     <row r="257" ht="13.5" customHeight="1">
-      <c r="A257" s="21"/>
+      <c r="A257" s="22"/>
       <c r="B257" s="4"/>
       <c r="C257" s="4"/>
       <c r="D257" s="4"/>
@@ -4060,7 +4104,7 @@
       <c r="H257" s="4"/>
     </row>
     <row r="258" ht="13.5" customHeight="1">
-      <c r="A258" s="21"/>
+      <c r="A258" s="22"/>
       <c r="B258" s="4"/>
       <c r="C258" s="4"/>
       <c r="D258" s="4"/>
@@ -4070,7 +4114,7 @@
       <c r="H258" s="4"/>
     </row>
     <row r="259" ht="13.5" customHeight="1">
-      <c r="A259" s="21"/>
+      <c r="A259" s="22"/>
       <c r="B259" s="4"/>
       <c r="C259" s="4"/>
       <c r="D259" s="4"/>
@@ -4080,7 +4124,7 @@
       <c r="H259" s="4"/>
     </row>
     <row r="260" ht="13.5" customHeight="1">
-      <c r="A260" s="21"/>
+      <c r="A260" s="22"/>
       <c r="B260" s="4"/>
       <c r="C260" s="4"/>
       <c r="D260" s="4"/>
@@ -4090,7 +4134,7 @@
       <c r="H260" s="4"/>
     </row>
     <row r="261" ht="13.5" customHeight="1">
-      <c r="A261" s="21"/>
+      <c r="A261" s="22"/>
       <c r="B261" s="4"/>
       <c r="C261" s="4"/>
       <c r="D261" s="4"/>
@@ -4100,7 +4144,7 @@
       <c r="H261" s="4"/>
     </row>
     <row r="262" ht="13.5" customHeight="1">
-      <c r="A262" s="21"/>
+      <c r="A262" s="22"/>
       <c r="B262" s="4"/>
       <c r="C262" s="4"/>
       <c r="D262" s="4"/>
@@ -4110,7 +4154,7 @@
       <c r="H262" s="4"/>
     </row>
     <row r="263" ht="13.5" customHeight="1">
-      <c r="A263" s="21"/>
+      <c r="A263" s="22"/>
       <c r="B263" s="4"/>
       <c r="C263" s="4"/>
       <c r="D263" s="4"/>
@@ -4120,7 +4164,7 @@
       <c r="H263" s="4"/>
     </row>
     <row r="264" ht="13.5" customHeight="1">
-      <c r="A264" s="21"/>
+      <c r="A264" s="22"/>
       <c r="B264" s="4"/>
       <c r="C264" s="4"/>
       <c r="D264" s="4"/>
@@ -4130,7 +4174,7 @@
       <c r="H264" s="4"/>
     </row>
     <row r="265" ht="13.5" customHeight="1">
-      <c r="A265" s="21"/>
+      <c r="A265" s="22"/>
       <c r="B265" s="4"/>
       <c r="C265" s="4"/>
       <c r="D265" s="4"/>
@@ -4584,13 +4628,13 @@
   </sheetViews>
   <sheetFormatPr defaultColWidth="12.6667" defaultRowHeight="15" customHeight="1" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
-    <col min="1" max="1" width="23.3516" style="22" customWidth="1"/>
-    <col min="2" max="5" width="9.35156" style="22" customWidth="1"/>
-    <col min="6" max="16384" width="12.6719" style="22" customWidth="1"/>
+    <col min="1" max="1" width="23.3516" style="23" customWidth="1"/>
+    <col min="2" max="5" width="9.35156" style="23" customWidth="1"/>
+    <col min="6" max="16384" width="12.6719" style="23" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" ht="13.5" customHeight="1">
-      <c r="A1" t="s" s="23">
+      <c r="A1" t="s" s="24">
         <v>5</v>
       </c>
       <c r="B1" s="4"/>
@@ -4627,7 +4671,7 @@
     </row>
     <row r="5" ht="13.5" customHeight="1">
       <c r="A5" t="s" s="19">
-        <v>24</v>
+        <v>26</v>
       </c>
       <c r="B5" s="4"/>
       <c r="C5" s="4"/>

</xml_diff>

<commit_message>
Fixed services, tests and row handlers
</commit_message>
<xml_diff>
--- a/backend/fms_core/tests/valid_templates/Project_link_samples_v4_0_0.xlsx
+++ b/backend/fms_core/tests/valid_templates/Project_link_samples_v4_0_0.xlsx
@@ -12,7 +12,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" uniqueCount="28">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" uniqueCount="29">
   <si>
     <t>Project link samples Template</t>
   </si>
@@ -96,6 +96,9 @@
   </si>
   <si>
     <t>B</t>
+  </si>
+  <si>
+    <t>1</t>
   </si>
 </sst>
 </file>
@@ -1673,7 +1676,9 @@
       <c r="C15" t="s" s="19">
         <v>27</v>
       </c>
-      <c r="D15" s="19"/>
+      <c r="D15" t="s" s="19">
+        <v>28</v>
+      </c>
       <c r="E15" t="s" s="19">
         <v>21</v>
       </c>

</xml_diff>

<commit_message>
Fixed error messages and tests.
</commit_message>
<xml_diff>
--- a/backend/fms_core/tests/valid_templates/Project_link_samples_v4_0_0.xlsx
+++ b/backend/fms_core/tests/valid_templates/Project_link_samples_v4_0_0.xlsx
@@ -53,7 +53,7 @@
     <t>Add to project</t>
   </si>
   <si>
-    <t>ProjectTest1</t>
+    <t>ProjectTest3</t>
   </si>
   <si>
     <t>SampleTestForLink1</t>
@@ -74,13 +74,13 @@
     <t>Remove from project</t>
   </si>
   <si>
-    <t>ProjectTest3</t>
-  </si>
-  <si>
     <t>SampleTestForUnlink</t>
   </si>
   <si>
     <t>CONTAINER4PROJECTLINKSAMPLES3</t>
+  </si>
+  <si>
+    <t>ProjectTest1</t>
   </si>
   <si>
     <t>Add to study</t>
@@ -1593,15 +1593,15 @@
         <v>19</v>
       </c>
       <c r="B11" t="s" s="19">
-        <v>20</v>
+        <v>13</v>
       </c>
       <c r="C11" s="4"/>
       <c r="D11" s="4"/>
       <c r="E11" t="s" s="19">
+        <v>20</v>
+      </c>
+      <c r="F11" t="s" s="19">
         <v>21</v>
-      </c>
-      <c r="F11" t="s" s="19">
-        <v>22</v>
       </c>
       <c r="G11" s="19"/>
       <c r="H11" s="4"/>
@@ -1611,7 +1611,7 @@
         <v>12</v>
       </c>
       <c r="B12" t="s" s="19">
-        <v>20</v>
+        <v>22</v>
       </c>
       <c r="C12" s="4"/>
       <c r="D12" s="4"/>
@@ -1629,7 +1629,7 @@
         <v>23</v>
       </c>
       <c r="B13" t="s" s="21">
-        <v>13</v>
+        <v>22</v>
       </c>
       <c r="C13" t="s" s="19">
         <v>24</v>
@@ -1649,7 +1649,7 @@
         <v>23</v>
       </c>
       <c r="B14" t="s" s="21">
-        <v>13</v>
+        <v>22</v>
       </c>
       <c r="C14" t="s" s="19">
         <v>24</v>
@@ -1671,7 +1671,7 @@
         <v>26</v>
       </c>
       <c r="B15" t="s" s="21">
-        <v>13</v>
+        <v>22</v>
       </c>
       <c r="C15" t="s" s="19">
         <v>27</v>
@@ -1680,10 +1680,10 @@
         <v>28</v>
       </c>
       <c r="E15" t="s" s="19">
+        <v>20</v>
+      </c>
+      <c r="F15" t="s" s="19">
         <v>21</v>
-      </c>
-      <c r="F15" t="s" s="19">
-        <v>22</v>
       </c>
       <c r="G15" s="19"/>
       <c r="H15" s="20"/>

</xml_diff>